<commit_message>
8Aug - 4Easy solutions
</commit_message>
<xml_diff>
--- a/progress_atHR.xlsx
+++ b/progress_atHR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venkatanitin\github\HackerRank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489EF4B2-7E32-4734-B609-B8D046AB5FB2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACDE3E7-C6F1-4F07-B6EE-CF1C9D637463}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5A338B89-5BFB-4824-BA99-AC87D7019335}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranking </t>
   </si>
 </sst>
 </file>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF128642-0414-45D0-B575-536F37B10590}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,6 +501,9 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
       <c r="E1" t="s">
         <v>27</v>
       </c>
@@ -571,8 +577,26 @@
         <v>28</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43685</v>
+      </c>
+      <c r="B8">
+        <v>132477</v>
+      </c>
+      <c r="C8">
+        <v>112720</v>
+      </c>
+      <c r="D8">
+        <v>126722</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -621,7 +645,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +673,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="2">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -754,7 +778,7 @@
       </c>
       <c r="B16" s="2">
         <f>SUM(B2:B14)</f>
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>